<commit_message>
Finish dict of QA
</commit_message>
<xml_diff>
--- a/Clustering/untitled.xlsx
+++ b/Clustering/untitled.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\World\Documents\SeniorProject\datast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\World\Documents\SeniorProject\datast\Clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98447B00-25C8-400E-BC5E-090ED5EB2D11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFBD712-A5DB-4C73-9F73-7267793C4208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ปี</t>
   </si>
@@ -43,18 +43,6 @@
   </si>
   <si>
     <t>พลังงานทดแทน</t>
-  </si>
-  <si>
-    <t>2559 </t>
-  </si>
-  <si>
-    <t>2560 </t>
-  </si>
-  <si>
-    <t>2561 </t>
-  </si>
-  <si>
-    <t>2562 </t>
   </si>
 </sst>
 </file>
@@ -435,7 +423,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -468,8 +456,8 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
+      <c r="A2">
+        <v>2559</v>
       </c>
       <c r="B2">
         <v>20296.86</v>
@@ -488,8 +476,8 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>7</v>
+      <c r="A3">
+        <v>2560</v>
       </c>
       <c r="B3">
         <v>17615.38</v>
@@ -508,8 +496,8 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>8</v>
+      <c r="A4">
+        <v>2561</v>
       </c>
       <c r="B4">
         <v>16062.72</v>
@@ -528,8 +516,8 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>9</v>
+      <c r="A5">
+        <v>2562</v>
       </c>
       <c r="B5">
         <v>17752.689999999999</v>

</xml_diff>